<commit_message>
issue of hwang is solved
</commit_message>
<xml_diff>
--- a/dataset/2nd_data/hwang/hwang_env_detail_data.xlsx
+++ b/dataset/2nd_data/hwang/hwang_env_detail_data.xlsx
@@ -6856,10 +6856,8 @@
       <c r="BO30" t="n">
         <v>0.5</v>
       </c>
-      <c r="BP30" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
+      <c r="BP30" t="n">
+        <v>0</v>
       </c>
       <c r="BQ30" t="n">
         <v>-1.9</v>
@@ -7055,10 +7053,8 @@
       <c r="BJ31" t="n">
         <v>17.99461682242996</v>
       </c>
-      <c r="BK31" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
+      <c r="BK31" t="n">
+        <v>0</v>
       </c>
       <c r="BL31" t="n">
         <v>17.99774193548387</v>
@@ -7069,15 +7065,11 @@
       <c r="BN31" t="n">
         <v>2.266666666666667</v>
       </c>
-      <c r="BO31" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
-      </c>
-      <c r="BP31" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
+      <c r="BO31" t="n">
+        <v>0</v>
+      </c>
+      <c r="BP31" t="n">
+        <v>0</v>
       </c>
       <c r="BQ31" t="n">
         <v>-2.609999999999999</v>
@@ -15977,10 +15969,8 @@
       <c r="BN73" t="n">
         <v>3.1</v>
       </c>
-      <c r="BO73" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
+      <c r="BO73" t="n">
+        <v>0</v>
       </c>
       <c r="BP73" t="n">
         <v>2.899999999999999</v>
@@ -16391,10 +16381,8 @@
       <c r="BJ75" t="n">
         <v>22.15617590822191</v>
       </c>
-      <c r="BK75" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
+      <c r="BK75" t="n">
+        <v>0</v>
       </c>
       <c r="BL75" t="n">
         <v>22.99011730205281</v>
@@ -16405,10 +16393,8 @@
       <c r="BN75" t="n">
         <v>2.466666666666667</v>
       </c>
-      <c r="BO75" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
+      <c r="BO75" t="n">
+        <v>0</v>
       </c>
       <c r="BP75" t="n">
         <v>2.81</v>
@@ -16619,10 +16605,8 @@
       <c r="BN76" t="n">
         <v>2.083333333333333</v>
       </c>
-      <c r="BO76" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
+      <c r="BO76" t="n">
+        <v>0</v>
       </c>
       <c r="BP76" t="n">
         <v>3.19</v>
@@ -20013,10 +19997,8 @@
       <c r="BN92" t="n">
         <v>3.266666666666667</v>
       </c>
-      <c r="BO92" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
+      <c r="BO92" t="n">
+        <v>0</v>
       </c>
       <c r="BP92" t="n">
         <v>1</v>

</xml_diff>